<commit_message>
commit to update tgw
</commit_message>
<xml_diff>
--- a/Vpc-TGW/TGW-RT-Understanding.xlsx
+++ b/Vpc-TGW/TGW-RT-Understanding.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26815"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCCA8AA9-8093-4131-A338-C4508CE5018F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F54CEB6-62DA-4FF1-A9CF-6A333D73B6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TGWRT" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,9 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="52">
   <si>
     <t>TGWRouteTable-for-SFDC</t>
   </si>
@@ -186,13 +189,14 @@
     <t>AND Edge Association with IGW</t>
   </si>
   <si>
-    <t>Important:
+    <t xml:space="preserve">Important:
 1. Assuming GWLB is already created by Firewalls.
 2. Create a Endpoint service for that GWLB and share it(without acceptance required) with all the Spoke Accounts.
 3. Create a IGW in Spoke Account.
 4. Create GWLBENP inside the Spoke Account for that Firewalls GWLB.
 4. Inside the spoke account go to VPC Main Route table and add routes for the GWLENP Subnets and do Edge Association with the Internet gateway.
-5. Do the required changes mentioned in here.</t>
+5. Do the required changes mentioned in here.
+6. IF Traffic is coming from different account or VPN, just add the Account CIDR in destination and Transit gateway as a target. this subnet will send the traffic to transit gateway for further routing for return route. </t>
   </si>
   <si>
     <t>LB Subnet CIDR - 1</t>
@@ -213,10 +217,19 @@
     <t>Route</t>
   </si>
   <si>
-    <t>Spoke Account LB SUBNET RT -1</t>
-  </si>
-  <si>
-    <t>Spoke Account LB SUBNET RT -2</t>
+    <t>Spoke Account LB SUBNET RT -1 - Public</t>
+  </si>
+  <si>
+    <t>Account-1 CIDR</t>
+  </si>
+  <si>
+    <t>Transit Gateway</t>
+  </si>
+  <si>
+    <t>VPN CIDR</t>
+  </si>
+  <si>
+    <t>Spoke Account LB SUBNET RT -2 - Public</t>
   </si>
   <si>
     <t>Spoke Account GWLBENP SUBNET RT -1</t>
@@ -426,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -444,6 +457,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -471,6 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B42" sqref="A38:B42"/>
     </sheetView>
   </sheetViews>
@@ -801,12 +818,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
     </row>
@@ -820,7 +837,7 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
@@ -830,7 +847,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="E3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
@@ -842,7 +859,7 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
@@ -854,7 +871,7 @@
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
@@ -866,7 +883,7 @@
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
@@ -878,21 +895,21 @@
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="E8" s="12"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="E9" s="12"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="E10" s="12"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
@@ -904,7 +921,7 @@
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
@@ -914,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="E12" s="12"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
@@ -926,7 +943,7 @@
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
@@ -938,7 +955,7 @@
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
@@ -950,21 +967,21 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="E16" s="12"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="E17" s="12"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="E18" s="12"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
@@ -1014,11 +1031,11 @@
       <c r="C23" s="1"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
@@ -1064,10 +1081,10 @@
       <c r="A30" s="6"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="14"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
@@ -1102,10 +1119,10 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="10"/>
+      <c r="B38" s="11"/>
       <c r="E38" t="s">
         <v>28</v>
       </c>
@@ -1149,10 +1166,10 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="10"/>
+      <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="4" t="s">
@@ -1171,10 +1188,10 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="10"/>
+      <c r="B48" s="11"/>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="4" t="s">
@@ -1193,10 +1210,10 @@
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="10"/>
+      <c r="B52" s="11"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="4" t="s">
@@ -1233,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AE55BF-C098-4795-B30E-46A1B4381B00}">
-  <dimension ref="A2:E28"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15"/>
@@ -1246,14 +1263,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="11"/>
       <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1264,7 +1281,7 @@
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
@@ -1273,7 +1290,7 @@
       <c r="B4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
@@ -1282,7 +1299,7 @@
       <c r="B5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
@@ -1291,17 +1308,17 @@
       <c r="B6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="E7" s="17"/>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="E8" s="17"/>
+      <c r="B8" s="11"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
@@ -1310,7 +1327,7 @@
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
@@ -1319,125 +1336,157 @@
       <c r="B10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="17"/>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="E12" s="17"/>
+      <c r="A12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="E13" s="17"/>
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="9" t="s">
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4" t="s">
+      <c r="B19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="11"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="8" t="s">
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
+      <c r="B24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4" t="s">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="8" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="5" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="E2:E18"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="E2:E17"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>